<commit_message>
added right path for navigation bar
</commit_message>
<xml_diff>
--- a/Additional Files/Zeiterfassung_MarcusMarohn_741986.xlsx
+++ b/Additional Files/Zeiterfassung_MarcusMarohn_741986.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -40,6 +40,30 @@
   </si>
   <si>
     <t>Gespräch mit dem "Kunden" über Use Cases und Features</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>Einarbeiten in Asp.net core Techniken</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Aufsetzen verschiedener Webprojekte, Austesten der MVC Struktur</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>Erste View Seiten erstellt</t>
+  </si>
+  <si>
+    <t>7h</t>
+  </si>
+  <si>
+    <t>Erste vollständige Verbindung von View -&gt; Controller -&gt; Datenbank hergestellt</t>
   </si>
 </sst>
 </file>
@@ -392,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +461,50 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42721</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42722</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42723</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42724</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added few gui elements, created class "Data" for all static data like school times, weekdays, etc.
</commit_message>
<xml_diff>
--- a/Additional Files/Zeiterfassung_MarcusMarohn_741986.xlsx
+++ b/Additional Files/Zeiterfassung_MarcusMarohn_741986.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Datum</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Erste vollständige Verbindung von View -&gt; Controller -&gt; Datenbank hergestellt</t>
+  </si>
+  <si>
+    <t>FullCalendar Komponente eingebunden</t>
+  </si>
+  <si>
+    <t>10h</t>
+  </si>
+  <si>
+    <t>Reservierungsvorgang erfolgreich implementiert</t>
   </si>
 </sst>
 </file>
@@ -416,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +514,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42726</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42727</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new course page
</commit_message>
<xml_diff>
--- a/Additional Files/Zeiterfassung_MarcusMarohn_741986.xlsx
+++ b/Additional Files/Zeiterfassung_MarcusMarohn_741986.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Reservierungsvorgang erfolgreich implementiert</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>Kleinere Anpassungen an der Oberfläche, Anzeigen der Kurse hinzugefügt, refactoring und Funktionalitäten im ViewModelbereich</t>
   </si>
 </sst>
 </file>
@@ -425,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C10"/>
+  <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,6 +542,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42732</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>